<commit_message>
Report Updated With File 2024-01-31
</commit_message>
<xml_diff>
--- a/Results/Серії без назв препаратів.xlsx
+++ b/Results/Серії без назв препаратів.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>08AR23034</t>
+          <t>1322</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -464,30 +464,6 @@
         </is>
       </c>
       <c r="B3" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2821X029B</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>62C21012A</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
         <is>
           <t>[]</t>
         </is>

</xml_diff>

<commit_message>
Data can be exported and loaded as .xlsx now! Also a 2024-02-06 update proceeded
</commit_message>
<xml_diff>
--- a/Results/Серії без назв препаратів.xlsx
+++ b/Results/Серії без назв препаратів.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,30 +445,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1322</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2821X029A</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Menu bar and unique facility names
Added menu bar. Facility names are now also unified using code->'most popular name' mapping.

Added facilities-presence testing file that uses official dataset of registered facilities and reports on which facilities there are not reporting.

Fixed some bugs (incorrect region name display in the stock infographics section due to translation issues)
</commit_message>
<xml_diff>
--- a/Results/Серії без назв препаратів.xlsx
+++ b/Results/Серії без назв препаратів.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,6 +445,18 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>68D23006A</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>